<commit_message>
remove some logic configurations
</commit_message>
<xml_diff>
--- a/Bin/resource/excel/Cost.xlsx
+++ b/Bin/resource/excel/Cost.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\ArkGameFrame\Bin\Server\DataConfig\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opensource\ARK.net_header\Bin\resource\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="27525" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="27525" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,8 +27,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -103,16 +103,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
@@ -124,148 +117,20 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -274,51 +139,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,203 +488,197 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
     <col min="6" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10" t="s">
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="13" t="s">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="14">
-        <v>0</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="14">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10">
         <v>100</v>
       </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A7" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:E6 B7:J7" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>